<commit_message>
Update: Latest Jira issues and integration improvements
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,9 +469,17 @@
           <t>TPGSOC-1346774</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:00:24.012-0500</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:05:42.215-0500</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -483,9 +491,17 @@
           <t>TPGSOC-1346749</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:45:24.794-0500</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:31:21.086-0500</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -497,9 +513,17 @@
           <t>TPGSOC-1346728</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:15:53.448-0500</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:20:41.719-0500</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -511,8 +535,16 @@
           <t>TPGSOC-1346665</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:35:47.674-0500</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:47:01.091-0500</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -525,9 +557,17 @@
           <t>TPGSOC-1346619</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:29:46.925-0500</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:30:08.186-0500</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -539,8 +579,16 @@
           <t>TPGSOC-1346039</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:34:53.684-0500</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2026-01-15T13:22:11.843-0500</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -553,7 +601,11 @@
           <t>TPGSOC-1346033</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:58:46.600-0500</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -567,7 +619,11 @@
           <t>TPGSOC-1345994</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2026-01-15T19:51:49.848-0500</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -581,8 +637,16 @@
           <t>TPGSOC-1345932</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:19:41.368-0500</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:55:35.561-0500</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -595,8 +659,16 @@
           <t>TPGSOC-1345924</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:11:15.402-0500</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:55:00.479-0500</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -609,8 +681,16 @@
           <t>TPGSOC-1345865</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-15T09:47:10.662-0500</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:04:52.006-0500</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -623,9 +703,17 @@
           <t>TPGSOC-1345860</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:38:21.744-0500</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:56:11.732-0500</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -637,7 +725,11 @@
           <t>TPGSOC-1345789</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-15T18:49:35.472-0500</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -651,8 +743,16 @@
           <t>TPGSOC-1345078</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-14T23:57:30.381-0500</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-15T00:32:42.229-0500</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -665,8 +765,16 @@
           <t>TPGSOC-1345038</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-14T23:42:10.594-0500</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:08:03.854-0500</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -679,8 +787,16 @@
           <t>TPGSOC-1344766</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-14T17:29:36.581-0500</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-14T20:46:57.091-0500</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -693,8 +809,16 @@
           <t>TPGSOC-1344746</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-14T15:29:24.568-0500</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:09:10.304-0500</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -707,9 +831,21 @@
           <t>TPGSOC-1344702</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-14T15:28:01.055-0500</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:06:00.051-0500</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:08:01.554-0500</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -789,8 +925,16 @@
           <t>TPGSOC-1344131</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-14T12:23:48.584-0500</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-01-14T20:47:23.431-0500</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
@@ -1889,9 +2033,21 @@
           <t>TPGSOC-1340674</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2026-01-11T15:12:33.149-0500</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2026-01-11T21:01:05.151-0500</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2026-01-11T21:05:53.010-0500</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
@@ -2883,8 +3039,16 @@
           <t>TPGSOC-1337015</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2026-01-07T13:26:07.581-0500</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:59:10.479-0500</t>
+        </is>
+      </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
@@ -2941,7 +3105,11 @@
           <t>2026-01-07T15:43:42.084-0500</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:09:50.333-0500</t>
+        </is>
+      </c>
       <c r="E85" t="inlineStr">
         <is>
           <t>2026-01-07T13:04:22.950-0500</t>
@@ -2957,7 +3125,11 @@
           <t>2.66</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>190.09</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3683,8 +3855,16 @@
           <t>TPGSOC-1330444</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2026-01-01T08:31:30.704-0500</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2026-01-01T09:04:50.071-0500</t>
+        </is>
+      </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
@@ -4113,8 +4293,16 @@
           <t>TPGSOC-1328791</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr"/>
-      <c r="C120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2025-12-31T06:10:53.768-0500</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2025-12-31T10:38:05.820-0500</t>
+        </is>
+      </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
@@ -4271,9 +4459,21 @@
           <t>TPGSOC-1328093</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:27:32.138-0500</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:12:53.621-0500</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:24:45.273-0500</t>
+        </is>
+      </c>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
@@ -4395,8 +4595,16 @@
           <t>TPGSOC-1327668</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2025-12-31T04:03:15.646-0500</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2025-12-31T10:37:56.064-0500</t>
+        </is>
+      </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
@@ -4443,8 +4651,16 @@
           <t>TPGSOC-1327100</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2025-12-29T08:49:51.016-0500</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2025-12-29T09:34:44.539-0500</t>
+        </is>
+      </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
@@ -4475,9 +4691,21 @@
           <t>TPGSOC-1324953</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
-      <c r="D133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>2025-12-27T07:43:51.377-0500</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2025-12-27T07:53:22.239-0500</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:57:05.462-0500</t>
+        </is>
+      </c>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
@@ -4573,9 +4801,21 @@
           <t>TPGSOC-1323444</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-      <c r="D136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>2025-12-29T07:07:36.908-0500</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2025-12-29T08:41:38.437-0500</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2025-12-26T19:46:09.269-0500</t>
+        </is>
+      </c>
       <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
@@ -4623,7 +4863,11 @@
           <t>2025-12-25T08:47:40.232-0500</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr"/>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2026-01-14T22:11:26.800-0500</t>
+        </is>
+      </c>
       <c r="E138" t="inlineStr">
         <is>
           <t>2025-12-25T05:11:21.178-0500</t>
@@ -4639,7 +4883,11 @@
           <t>3.61</t>
         </is>
       </c>
-      <c r="H138" t="inlineStr"/>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>497.00</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5277,7 +5525,11 @@
           <t>2025-12-22T08:32:05.848-0500</t>
         </is>
       </c>
-      <c r="D157" t="inlineStr"/>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2026-01-14T22:08:27.542-0500</t>
+        </is>
+      </c>
       <c r="E157" t="inlineStr">
         <is>
           <t>2025-12-22T01:49:37.979-0500</t>
@@ -5293,7 +5545,11 @@
           <t>6.71</t>
         </is>
       </c>
-      <c r="H157" t="inlineStr"/>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>572.31</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6072,312 +6328,6 @@
         </is>
       </c>
       <c r="H178" t="inlineStr"/>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>TPGSOC-1314437</t>
-        </is>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>2025-12-17T04:53:54.678-0500</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr"/>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>2025-12-19T09:34:53.580-0500</t>
-        </is>
-      </c>
-      <c r="E179" t="inlineStr">
-        <is>
-          <t>2025-12-17T04:55:23.585-0500</t>
-        </is>
-      </c>
-      <c r="F179" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" t="inlineStr">
-        <is>
-          <t>52.66</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>TPGSOC-1314418</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>2025-12-16T23:47:41.739-0500</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>2025-12-17T07:14:31.502-0500</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>2025-12-19T05:04:13.387-0500</t>
-        </is>
-      </c>
-      <c r="E180" t="inlineStr">
-        <is>
-          <t>2025-12-16T23:59:43.202-0500</t>
-        </is>
-      </c>
-      <c r="F180" t="inlineStr">
-        <is>
-          <t>0.20</t>
-        </is>
-      </c>
-      <c r="G180" t="inlineStr">
-        <is>
-          <t>7.25</t>
-        </is>
-      </c>
-      <c r="H180" t="inlineStr">
-        <is>
-          <t>53.08</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>TPGSOC-1314037</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>2025-12-16T08:32:46.979-0500</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>2025-12-16T09:42:25.005-0500</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>2026-01-07T09:47:33.379-0500</t>
-        </is>
-      </c>
-      <c r="E181" t="inlineStr">
-        <is>
-          <t>2025-12-16T08:36:43.283-0500</t>
-        </is>
-      </c>
-      <c r="F181" t="inlineStr">
-        <is>
-          <t>0.07</t>
-        </is>
-      </c>
-      <c r="G181" t="inlineStr">
-        <is>
-          <t>1.09</t>
-        </is>
-      </c>
-      <c r="H181" t="inlineStr">
-        <is>
-          <t>529.18</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>TPGSOC-1313430</t>
-        </is>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>2025-12-16T02:21:38.497-0500</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr"/>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>2025-12-16T12:02:20.933-0500</t>
-        </is>
-      </c>
-      <c r="E182" t="inlineStr">
-        <is>
-          <t>2025-12-16T02:27:09.410-0500</t>
-        </is>
-      </c>
-      <c r="F182" t="inlineStr">
-        <is>
-          <t>0.09</t>
-        </is>
-      </c>
-      <c r="G182" t="inlineStr"/>
-      <c r="H182" t="inlineStr">
-        <is>
-          <t>9.59</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>TPGSOC-1313265</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr"/>
-      <c r="C183" t="inlineStr"/>
-      <c r="D183" t="inlineStr"/>
-      <c r="E183" t="inlineStr"/>
-      <c r="F183" t="inlineStr"/>
-      <c r="G183" t="inlineStr"/>
-      <c r="H183" t="inlineStr"/>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312987</t>
-        </is>
-      </c>
-      <c r="B184" t="inlineStr"/>
-      <c r="C184" t="inlineStr"/>
-      <c r="D184" t="inlineStr"/>
-      <c r="E184" t="inlineStr"/>
-      <c r="F184" t="inlineStr"/>
-      <c r="G184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312963</t>
-        </is>
-      </c>
-      <c r="B185" t="inlineStr"/>
-      <c r="C185" t="inlineStr"/>
-      <c r="D185" t="inlineStr"/>
-      <c r="E185" t="inlineStr"/>
-      <c r="F185" t="inlineStr"/>
-      <c r="G185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312942</t>
-        </is>
-      </c>
-      <c r="B186" t="inlineStr"/>
-      <c r="C186" t="inlineStr"/>
-      <c r="D186" t="inlineStr"/>
-      <c r="E186" t="inlineStr"/>
-      <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312808</t>
-        </is>
-      </c>
-      <c r="B187" t="inlineStr"/>
-      <c r="C187" t="inlineStr"/>
-      <c r="D187" t="inlineStr"/>
-      <c r="E187" t="inlineStr"/>
-      <c r="F187" t="inlineStr"/>
-      <c r="G187" t="inlineStr"/>
-      <c r="H187" t="inlineStr"/>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312692</t>
-        </is>
-      </c>
-      <c r="B188" t="inlineStr"/>
-      <c r="C188" t="inlineStr"/>
-      <c r="D188" t="inlineStr"/>
-      <c r="E188" t="inlineStr"/>
-      <c r="F188" t="inlineStr"/>
-      <c r="G188" t="inlineStr"/>
-      <c r="H188" t="inlineStr"/>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312688</t>
-        </is>
-      </c>
-      <c r="B189" t="inlineStr"/>
-      <c r="C189" t="inlineStr"/>
-      <c r="D189" t="inlineStr"/>
-      <c r="E189" t="inlineStr"/>
-      <c r="F189" t="inlineStr"/>
-      <c r="G189" t="inlineStr"/>
-      <c r="H189" t="inlineStr"/>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312520</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr"/>
-      <c r="C190" t="inlineStr"/>
-      <c r="D190" t="inlineStr"/>
-      <c r="E190" t="inlineStr"/>
-      <c r="F190" t="inlineStr"/>
-      <c r="G190" t="inlineStr"/>
-      <c r="H190" t="inlineStr"/>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312327</t>
-        </is>
-      </c>
-      <c r="B191" t="inlineStr"/>
-      <c r="C191" t="inlineStr"/>
-      <c r="D191" t="inlineStr"/>
-      <c r="E191" t="inlineStr"/>
-      <c r="F191" t="inlineStr"/>
-      <c r="G191" t="inlineStr"/>
-      <c r="H191" t="inlineStr"/>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312250</t>
-        </is>
-      </c>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
-      <c r="D192" t="inlineStr"/>
-      <c r="E192" t="inlineStr"/>
-      <c r="F192" t="inlineStr"/>
-      <c r="G192" t="inlineStr"/>
-      <c r="H192" t="inlineStr"/>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>TPGSOC-1312078</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
-      <c r="D193" t="inlineStr"/>
-      <c r="E193" t="inlineStr"/>
-      <c r="F193" t="inlineStr"/>
-      <c r="G193" t="inlineStr"/>
-      <c r="H193" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Agregar logging detallado para diagnosticar problemas de changelog en GitHub Actions
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H178"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,9 +469,17 @@
           <t>TPGSOC-1346774</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:00:24.012-0500</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:05:42.215-0500</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -483,9 +491,17 @@
           <t>TPGSOC-1346749</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:45:24.794-0500</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:31:21.086-0500</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -497,9 +513,17 @@
           <t>TPGSOC-1346728</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:15:53.448-0500</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:20:41.719-0500</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -511,8 +535,16 @@
           <t>TPGSOC-1346665</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:35:47.674-0500</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:47:01.091-0500</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -525,9 +557,17 @@
           <t>TPGSOC-1346619</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:29:46.925-0500</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2026-01-15T16:30:08.186-0500</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -539,8 +579,16 @@
           <t>TPGSOC-1346039</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:34:53.684-0500</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2026-01-15T13:22:11.843-0500</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -553,9 +601,17 @@
           <t>TPGSOC-1346033</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2026-01-15T12:58:46.600-0500</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2026-01-15T23:25:19.335-0500</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -567,9 +623,17 @@
           <t>TPGSOC-1345994</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2026-01-15T19:51:49.848-0500</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2026-01-15T23:20:11.094-0500</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -581,8 +645,16 @@
           <t>TPGSOC-1345932</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:19:41.368-0500</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:55:35.561-0500</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -595,8 +667,16 @@
           <t>TPGSOC-1345924</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:11:15.402-0500</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:55:00.479-0500</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -609,8 +689,16 @@
           <t>TPGSOC-1345865</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-15T09:47:10.662-0500</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2026-01-15T10:04:52.006-0500</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -623,9 +711,17 @@
           <t>TPGSOC-1345860</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:38:21.744-0500</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2026-01-15T15:56:11.732-0500</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -637,9 +733,17 @@
           <t>TPGSOC-1345789</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-15T18:49:35.472-0500</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2026-01-15T23:32:57.207-0500</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -651,8 +755,16 @@
           <t>TPGSOC-1345078</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-14T23:57:30.381-0500</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-15T00:32:42.229-0500</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -665,8 +777,16 @@
           <t>TPGSOC-1345038</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-14T23:42:10.594-0500</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-15T01:08:03.854-0500</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -679,9 +799,21 @@
           <t>TPGSOC-1344766</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-14T17:29:36.581-0500</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-14T20:46:57.091-0500</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2026-01-15T23:25:30.360-0500</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -693,8 +825,16 @@
           <t>TPGSOC-1344746</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-14T15:29:24.568-0500</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:09:10.304-0500</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -707,9 +847,21 @@
           <t>TPGSOC-1344702</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-14T15:28:01.055-0500</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:06:00.051-0500</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2026-01-14T19:08:01.554-0500</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -721,8 +873,16 @@
           <t>TPGSOC-1344260</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-14T05:56:15.665-0500</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-14T07:04:58.133-0500</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -735,9 +895,17 @@
           <t>TPGSOC-1344137</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-14T03:43:51.483-0500</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2026-01-14T06:47:43.241-0500</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -749,9 +917,21 @@
           <t>TPGSOC-1344131</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-14T12:23:48.584-0500</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2026-01-14T20:47:23.431-0500</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2026-01-15T23:25:43.684-0500</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -763,8 +943,16 @@
           <t>TPGSOC-1343694</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-14T09:43:27.172-0500</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-14T13:57:38.871-0500</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
@@ -777,8 +965,16 @@
           <t>TPGSOC-1343496</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:08:45.433-0500</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2026-01-14T15:19:57.498-0500</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
@@ -791,8 +987,16 @@
           <t>TPGSOC-1343472</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-14T04:54:49.366-0500</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-14T06:29:58.978-0500</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
@@ -805,8 +1009,16 @@
           <t>TPGSOC-1343443</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-14T01:13:06.394-0500</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-14T02:41:46.414-0500</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
@@ -819,8 +1031,16 @@
           <t>TPGSOC-1343422</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2026-01-14T04:30:31.743-0500</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2026-01-14T06:39:31.017-0500</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -833,9 +1053,17 @@
           <t>TPGSOC-1343308</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:58:45.354-0500</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2026-01-13T13:16:55.599-0500</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -847,9 +1075,17 @@
           <t>TPGSOC-1343279</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:45:43.235-0500</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2026-01-13T16:55:34.709-0500</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -861,8 +1097,16 @@
           <t>TPGSOC-1343270</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2026-01-13T20:51:44.213-0500</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2026-01-13T21:41:31.788-0500</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -875,9 +1119,17 @@
           <t>TPGSOC-1343201</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2026-01-13T11:29:08.007-0500</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2026-01-13T13:13:00.509-0500</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -889,9 +1141,17 @@
           <t>TPGSOC-1343200</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2026-01-13T11:29:03.774-0500</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2026-01-13T13:07:20.190-0500</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -903,9 +1163,17 @@
           <t>TPGSOC-1343168</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2026-01-13T10:58:40.684-0500</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:57:50.544-0500</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -917,9 +1185,17 @@
           <t>TPGSOC-1343167</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2026-01-13T10:58:38.417-0500</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:46:59.480-0500</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -931,9 +1207,17 @@
           <t>TPGSOC-1343124</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2026-01-13T10:13:42.207-0500</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:43:39.175-0500</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -945,9 +1229,17 @@
           <t>TPGSOC-1343102</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2026-01-13T10:00:53.556-0500</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:37:08.668-0500</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -959,8 +1251,16 @@
           <t>TPGSOC-1343059</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2026-01-13T09:50:41.051-0500</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2026-01-13T14:45:02.741-0500</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
@@ -973,8 +1273,16 @@
           <t>TPGSOC-1343033</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2026-01-13T09:41:52.138-0500</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2026-01-13T13:30:49.942-0500</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
@@ -987,9 +1295,21 @@
           <t>TPGSOC-1343013</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2026-01-13T08:58:49.272-0500</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2026-01-13T11:15:28.210-0500</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2026-01-14T11:56:58.111-0500</t>
+        </is>
+      </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1001,9 +1321,21 @@
           <t>TPGSOC-1343007</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2026-01-13T08:58:32.920-0500</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2026-01-13T10:59:16.447-0500</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2026-01-14T11:41:31.811-0500</t>
+        </is>
+      </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1015,8 +1347,16 @@
           <t>TPGSOC-1342995</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2026-01-13T09:26:54.866-0500</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2026-01-13T12:05:46.346-0500</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
@@ -1029,8 +1369,16 @@
           <t>TPGSOC-1342952</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2026-01-13T08:39:21.602-0500</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2026-01-13T11:50:54.405-0500</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
@@ -1043,9 +1391,17 @@
           <t>TPGSOC-1342895</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2026-01-13T07:13:38.315-0500</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2026-01-13T09:38:18.475-0500</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
@@ -1057,9 +1413,21 @@
           <t>TPGSOC-1342891</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2026-01-13T07:13:14.139-0500</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2026-01-13T09:24:08.315-0500</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2026-01-14T11:29:57.762-0500</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -1071,9 +1439,17 @@
           <t>TPGSOC-1342873</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2026-01-13T06:58:15.503-0500</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2026-01-13T08:46:09.957-0500</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -1085,9 +1461,17 @@
           <t>TPGSOC-1342723</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2026-01-13T03:58:25.573-0500</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2026-01-13T05:33:34.630-0500</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -1099,9 +1483,21 @@
           <t>TPGSOC-1341440</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2026-01-12T11:14:57.034-0500</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2026-01-12T13:28:40.513-0500</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2026-01-14T11:24:33.964-0500</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
@@ -1113,9 +1509,17 @@
           <t>TPGSOC-1341368</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2026-01-12T07:58:12.795-0500</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2026-01-12T11:32:18.839-0500</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
@@ -1127,9 +1531,17 @@
           <t>TPGSOC-1341263</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2026-01-12T04:56:14.105-0500</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2026-01-12T05:46:45.285-0500</t>
+        </is>
+      </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
@@ -1141,9 +1553,17 @@
           <t>TPGSOC-1341248</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2026-01-12T04:39:41.294-0500</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2026-01-12T05:45:42.676-0500</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
@@ -1155,9 +1575,17 @@
           <t>TPGSOC-1341244</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2026-01-12T04:34:10.526-0500</t>
+        </is>
+      </c>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2026-01-12T05:43:04.006-0500</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
@@ -1169,8 +1597,16 @@
           <t>TPGSOC-1340785</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2026-01-12T06:59:03.874-0500</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2026-01-12T09:06:21.738-0500</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
@@ -1183,8 +1619,16 @@
           <t>TPGSOC-1340699</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2026-01-12T06:31:20.440-0500</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2026-01-12T11:14:18.449-0500</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
@@ -1197,9 +1641,21 @@
           <t>TPGSOC-1340674</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2026-01-11T15:12:33.149-0500</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2026-01-11T21:01:05.151-0500</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2026-01-11T21:05:53.010-0500</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
@@ -1208,11 +1664,19 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TPGSOC-1340670</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
+          <t>TPGSOC-1340673</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2026-01-11T15:12:31.184-0500</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2026-01-11T21:00:38.389-0500</t>
+        </is>
+      </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
@@ -1222,7 +1686,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TPGSOC-1340419</t>
+          <t>TPGSOC-1340670</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1236,12 +1700,24 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>TPGSOC-1340418</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
+          <t>TPGSOC-1340419</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2026-01-11T09:56:05.091-0500</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2026-01-11T14:18:14.956-0500</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2026-01-14T11:20:08.072-0500</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
@@ -1250,11 +1726,19 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>TPGSOC-1340417</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
+          <t>TPGSOC-1340418</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2026-01-11T07:19:35.106-0500</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2026-01-11T08:18:50.192-0500</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
@@ -1264,12 +1748,24 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>TPGSOC-1340378</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+          <t>TPGSOC-1340417</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2026-01-11T04:30:06.231-0500</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2026-01-11T05:40:34.605-0500</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:52:02.840-0500</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
@@ -1278,11 +1774,19 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TPGSOC-1340348</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
+          <t>TPGSOC-1340378</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2026-01-11T08:22:39.666-0500</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2026-01-11T13:17:13.251-0500</t>
+        </is>
+      </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
@@ -1292,7 +1796,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>TPGSOC-1339546</t>
+          <t>TPGSOC-1340348</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1306,12 +1810,20 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TPGSOC-1339529</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
+          <t>TPGSOC-1339546</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2026-01-09T20:02:45.767-0500</t>
+        </is>
+      </c>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2026-01-09T21:36:51.369-0500</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
@@ -1320,12 +1832,20 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>TPGSOC-1339395</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr"/>
+          <t>TPGSOC-1339529</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2026-01-09T19:41:51.365-0500</t>
+        </is>
+      </c>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2026-01-09T21:33:46.243-0500</t>
+        </is>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
@@ -1334,12 +1854,24 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>TPGSOC-1339204</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+          <t>TPGSOC-1339395</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2026-01-10T06:13:29.517-0500</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2026-01-10T06:18:40.095-0500</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:53:03.998-0500</t>
+        </is>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
@@ -1348,12 +1880,24 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>TPGSOC-1339107</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+          <t>TPGSOC-1339204</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2026-01-09T11:12:19.846-0500</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2026-01-09T12:43:23.423-0500</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2026-01-10T10:33:12.020-0500</t>
+        </is>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
@@ -1362,12 +1906,20 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TPGSOC-1339091</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
+          <t>TPGSOC-1339107</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2026-01-09T09:26:18.183-0500</t>
+        </is>
+      </c>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2026-01-09T11:24:32.994-0500</t>
+        </is>
+      </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
@@ -1376,12 +1928,24 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>TPGSOC-1339087</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+          <t>TPGSOC-1339091</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2026-01-09T09:13:53.383-0500</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2026-01-09T13:03:29.851-0500</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2026-01-10T10:30:08.192-0500</t>
+        </is>
+      </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
@@ -1390,12 +1954,20 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>TPGSOC-1338954</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
+          <t>TPGSOC-1339087</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2026-01-09T09:11:48.966-0500</t>
+        </is>
+      </c>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2026-01-09T11:21:24.712-0500</t>
+        </is>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
@@ -1404,12 +1976,20 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>TPGSOC-1338940</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
+          <t>TPGSOC-1338954</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2026-01-09T05:08:27.425-0500</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:07:39.671-0500</t>
+        </is>
+      </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
@@ -1418,12 +1998,24 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>TPGSOC-1338905</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
+          <t>TPGSOC-1338940</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2026-01-09T05:00:35.665-0500</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:44:09.805-0500</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2026-01-14T03:17:20.913-0500</t>
+        </is>
+      </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
@@ -1432,12 +2024,20 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TPGSOC-1338888</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
+          <t>TPGSOC-1338905</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2026-01-09T03:58:00.542-0500</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:48:53.307-0500</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
@@ -1446,12 +2046,20 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TPGSOC-1338839</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
+          <t>TPGSOC-1338888</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2026-01-09T03:37:57.910-0500</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:48:19.457-0500</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
@@ -1460,12 +2068,20 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>TPGSOC-1338829</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
+          <t>TPGSOC-1338839</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2026-01-09T02:36:50.739-0500</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:46:29.587-0500</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
@@ -1474,12 +2090,20 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>TPGSOC-1338368</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr"/>
+          <t>TPGSOC-1338829</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2026-01-09T02:13:21.716-0500</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2026-01-09T08:47:01.299-0500</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
@@ -1488,11 +2112,19 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>TPGSOC-1338112</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
+          <t>TPGSOC-1338368</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:42:26.201-0500</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2026-01-08T16:39:57.675-0500</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
@@ -1502,11 +2134,19 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>TPGSOC-1338033</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
+          <t>TPGSOC-1338112</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2026-01-08T10:43:42.404-0500</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2026-01-08T12:02:10.906-0500</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
@@ -1516,11 +2156,19 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>TPGSOC-1338032</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
+          <t>TPGSOC-1338033</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2026-01-08T10:10:57.376-0500</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2026-01-08T12:49:09.478-0500</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
@@ -1530,11 +2178,19 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>TPGSOC-1337947</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr"/>
+          <t>TPGSOC-1338032</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2026-01-08T09:56:57.034-0500</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2026-01-08T11:27:25.952-0500</t>
+        </is>
+      </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
@@ -1544,11 +2200,19 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>TPGSOC-1337159</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
+          <t>TPGSOC-1337947</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2026-01-08T09:33:09.525-0500</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2026-01-09T00:34:43.109-0500</t>
+        </is>
+      </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
@@ -1558,12 +2222,20 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>TPGSOC-1337149</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
+          <t>TPGSOC-1337159</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2026-01-07T19:36:00.781-0500</t>
+        </is>
+      </c>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2026-01-08T07:43:37.775-0500</t>
+        </is>
+      </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
@@ -1572,11 +2244,19 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TPGSOC-1337046</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
+          <t>TPGSOC-1337149</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2026-01-07T19:22:03.840-0500</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2026-01-08T05:28:20.706-0500</t>
+        </is>
+      </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
@@ -1586,12 +2266,24 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>TPGSOC-1337033</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+          <t>TPGSOC-1337046</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:49:32.015-0500</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2026-01-08T05:11:43.199-0500</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2026-01-14T13:30:59.921-0500</t>
+        </is>
+      </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
@@ -1600,12 +2292,24 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>TPGSOC-1337015</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+          <t>TPGSOC-1337033</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2026-01-08T05:04:24.190-0500</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2026-01-08T05:52:29.682-0500</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2026-01-14T03:16:33.673-0500</t>
+        </is>
+      </c>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
@@ -1614,11 +2318,19 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>TPGSOC-1337011</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
+          <t>TPGSOC-1337015</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2026-01-07T13:26:07.581-0500</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:59:10.479-0500</t>
+        </is>
+      </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
@@ -1628,11 +2340,19 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>TPGSOC-1336989</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
+          <t>TPGSOC-1337011</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2026-01-07T13:24:13.824-0500</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:28:32.714-0500</t>
+        </is>
+      </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
@@ -1642,12 +2362,24 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>TPGSOC-1336988</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+          <t>TPGSOC-1336989</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2026-01-07T12:43:02.806-0500</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2026-01-07T15:43:42.084-0500</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2026-01-15T11:09:50.333-0500</t>
+        </is>
+      </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
@@ -1656,12 +2388,24 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>TPGSOC-1336987</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+          <t>TPGSOC-1336988</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2026-01-07T12:40:09.605-0500</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:16:27.886-0500</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:54:49.653-0500</t>
+        </is>
+      </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
@@ -1670,12 +2414,24 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>TPGSOC-1336985</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+          <t>TPGSOC-1336987</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2026-01-07T12:36:49.099-0500</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:13:50.946-0500</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:55:45.093-0500</t>
+        </is>
+      </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
@@ -1684,12 +2440,20 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>TPGSOC-1336031</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
+          <t>TPGSOC-1336985</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2026-01-08T01:06:18.839-0500</t>
+        </is>
+      </c>
       <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2026-01-08T18:32:32.708-0500</t>
+        </is>
+      </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
@@ -1698,11 +2462,19 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>TPGSOC-1335970</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
+          <t>TPGSOC-1336031</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2026-01-06T20:19:16.238-0500</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2026-01-07T07:56:19.895-0500</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
@@ -1712,11 +2484,19 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>TPGSOC-1335915</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
+          <t>TPGSOC-1335970</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2026-01-06T18:48:57.060-0500</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2026-01-08T21:36:30.303-0500</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
@@ -1726,12 +2506,24 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>TPGSOC-1335859</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
+          <t>TPGSOC-1335915</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2026-01-06T17:23:54.712-0500</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2026-01-07T07:40:51.539-0500</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2026-01-14T03:14:29.137-0500</t>
+        </is>
+      </c>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
@@ -1740,12 +2532,20 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>TPGSOC-1335680</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
+          <t>TPGSOC-1335859</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2026-01-06T15:54:44.939-0500</t>
+        </is>
+      </c>
       <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2026-01-07T07:36:48.055-0500</t>
+        </is>
+      </c>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
@@ -1754,11 +2554,19 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>TPGSOC-1335561</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
+          <t>TPGSOC-1335680</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:43:37.280-0500</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2026-01-07T08:14:35.945-0500</t>
+        </is>
+      </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr"/>
@@ -1768,11 +2576,19 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>TPGSOC-1335454</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
+          <t>TPGSOC-1335561</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2026-01-06T12:51:06.539-0500</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2026-01-07T14:51:06.974-0500</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
@@ -1782,11 +2598,19 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TPGSOC-1335317</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
+          <t>TPGSOC-1335454</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2026-01-06T10:24:38.898-0500</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2026-01-06T13:17:45.492-0500</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr"/>
@@ -1796,11 +2620,19 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>TPGSOC-1335217</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
+          <t>TPGSOC-1335317</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2026-01-06T08:56:32.573-0500</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2026-01-06T11:15:33.566-0500</t>
+        </is>
+      </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
@@ -1810,12 +2642,24 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>TPGSOC-1334973</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+          <t>TPGSOC-1335217</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2026-01-06T06:59:17.026-0500</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2026-01-06T10:43:36.215-0500</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:37:26.623-0500</t>
+        </is>
+      </c>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
@@ -1824,11 +2668,19 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TPGSOC-1334361</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
+          <t>TPGSOC-1334973</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2026-01-06T02:00:33.694-0500</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2026-01-06T08:46:30.177-0500</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr"/>
@@ -1838,12 +2690,20 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>TPGSOC-1334250</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
+          <t>TPGSOC-1334361</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2026-01-05T17:35:37.919-0500</t>
+        </is>
+      </c>
       <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2026-01-06T02:11:03.202-0500</t>
+        </is>
+      </c>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
@@ -1852,12 +2712,24 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>TPGSOC-1334202</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+          <t>TPGSOC-1334265</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2026-01-06T07:22:55.837-0500</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2026-01-06T07:22:59.637-0500</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2026-01-06T07:23:18.511-0500</t>
+        </is>
+      </c>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
@@ -1866,12 +2738,24 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>TPGSOC-1332205</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+          <t>TPGSOC-1334250</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2026-01-05T15:54:16.032-0500</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2026-01-08T21:37:05.382-0500</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2026-01-14T13:25:25.696-0500</t>
+        </is>
+      </c>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
@@ -1880,7 +2764,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>TPGSOC-1332079</t>
+          <t>TPGSOC-1334202</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -1894,12 +2778,16 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>TPGSOC-1331677</t>
+          <t>TPGSOC-1332205</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:34:01.967-0500</t>
+        </is>
+      </c>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
@@ -1908,12 +2796,20 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>TPGSOC-1331559</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr"/>
+          <t>TPGSOC-1332079</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2026-01-03T07:17:51.200-0500</t>
+        </is>
+      </c>
       <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2026-01-03T11:43:45.596-0500</t>
+        </is>
+      </c>
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr"/>
@@ -1922,12 +2818,24 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>TPGSOC-1331531</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
+          <t>TPGSOC-1331677</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2026-01-04T06:30:43.846-0500</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2026-01-04T12:37:24.986-0500</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:27:09.158-0500</t>
+        </is>
+      </c>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
@@ -1936,12 +2844,24 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>TPGSOC-1330444</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+          <t>TPGSOC-1331559</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2026-01-03T07:00:40.259-0500</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2026-01-03T08:40:21.921-0500</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2026-01-03T09:14:23.326-0500</t>
+        </is>
+      </c>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
@@ -1950,7 +2870,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>TPGSOC-1329967</t>
+          <t>TPGSOC-1331531</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -1964,11 +2884,19 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>TPGSOC-1329925</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" t="inlineStr"/>
+          <t>TPGSOC-1330444</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2026-01-01T08:31:30.704-0500</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2026-01-01T09:04:50.071-0500</t>
+        </is>
+      </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
@@ -1978,12 +2906,20 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>TPGSOC-1329893</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr"/>
+          <t>TPGSOC-1329967</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2025-12-31T14:44:56.932-0500</t>
+        </is>
+      </c>
       <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2025-12-31T14:56:40.643-0500</t>
+        </is>
+      </c>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
@@ -1992,12 +2928,24 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>TPGSOC-1329858</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
+          <t>TPGSOC-1329925</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2025-12-31T14:42:50.519-0500</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2025-12-31T14:54:09.900-0500</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2026-01-07T09:42:54.464-0500</t>
+        </is>
+      </c>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
@@ -2006,12 +2954,20 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>TPGSOC-1329319</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr"/>
+          <t>TPGSOC-1329893</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>2025-12-31T12:43:54.234-0500</t>
+        </is>
+      </c>
       <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2025-12-31T12:47:59.586-0500</t>
+        </is>
+      </c>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
@@ -2020,12 +2976,20 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>TPGSOC-1329200</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr"/>
+          <t>TPGSOC-1329858</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2025-12-31T11:43:30.205-0500</t>
+        </is>
+      </c>
       <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2025-12-31T12:17:36.120-0500</t>
+        </is>
+      </c>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
@@ -2034,12 +2998,20 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>TPGSOC-1329074</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr"/>
+          <t>TPGSOC-1329319</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2025-12-31T02:21:22.981-0500</t>
+        </is>
+      </c>
       <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:49:23.835-0500</t>
+        </is>
+      </c>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
@@ -2048,11 +3020,19 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>TPGSOC-1329073</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
+          <t>TPGSOC-1329200</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>2025-12-30T19:15:15.375-0500</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2025-12-30T22:13:01.968-0500</t>
+        </is>
+      </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
@@ -2062,12 +3042,20 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>TPGSOC-1329072</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr"/>
+          <t>TPGSOC-1329074</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>2025-12-30T17:43:45.085-0500</t>
+        </is>
+      </c>
       <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr"/>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:33:54.988-0500</t>
+        </is>
+      </c>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
@@ -2076,12 +3064,20 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>TPGSOC-1328985</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr"/>
+          <t>TPGSOC-1329073</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2025-12-30T17:36:23.863-0500</t>
+        </is>
+      </c>
       <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr"/>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:34:17.845-0500</t>
+        </is>
+      </c>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
@@ -2090,12 +3086,20 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>TPGSOC-1328984</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr"/>
+          <t>TPGSOC-1329072</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2025-12-30T17:32:42.538-0500</t>
+        </is>
+      </c>
       <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr"/>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:34:40.416-0500</t>
+        </is>
+      </c>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
@@ -2104,12 +3108,20 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>TPGSOC-1328983</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr"/>
+          <t>TPGSOC-1328985</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>2025-12-30T15:26:47.177-0500</t>
+        </is>
+      </c>
       <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr"/>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:34:51.973-0500</t>
+        </is>
+      </c>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr"/>
@@ -2118,12 +3130,20 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>TPGSOC-1328791</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr"/>
+          <t>TPGSOC-1328984</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2025-12-30T15:24:17.542-0500</t>
+        </is>
+      </c>
       <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr"/>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:35:15.131-0500</t>
+        </is>
+      </c>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr"/>
@@ -2132,12 +3152,20 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>TPGSOC-1328786</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr"/>
+          <t>TPGSOC-1328983</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>2025-12-30T15:19:29.209-0500</t>
+        </is>
+      </c>
       <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2026-01-08T14:35:24.773-0500</t>
+        </is>
+      </c>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
       <c r="G121" t="inlineStr"/>
@@ -2146,11 +3174,19 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>TPGSOC-1328101</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
+          <t>TPGSOC-1328791</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2025-12-31T06:10:53.768-0500</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2025-12-31T10:38:05.820-0500</t>
+        </is>
+      </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
@@ -2160,12 +3196,24 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>TPGSOC-1328098</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr"/>
+          <t>TPGSOC-1328786</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2025-12-30T12:08:38.974-0500</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2025-12-30T12:42:06.804-0500</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2026-01-07T09:41:37.713-0500</t>
+        </is>
+      </c>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
       <c r="G123" t="inlineStr"/>
@@ -2174,12 +3222,20 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>TPGSOC-1328094</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr"/>
+          <t>TPGSOC-1328101</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:30:01.742-0500</t>
+        </is>
+      </c>
       <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr"/>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:18:03.112-0500</t>
+        </is>
+      </c>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
@@ -2188,12 +3244,20 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>TPGSOC-1328093</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr"/>
+          <t>TPGSOC-1328098</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:27:50.949-0500</t>
+        </is>
+      </c>
       <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:14:11.709-0500</t>
+        </is>
+      </c>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
@@ -2202,12 +3266,20 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>TPGSOC-1328090</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr"/>
+          <t>TPGSOC-1328094</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:27:37.326-0500</t>
+        </is>
+      </c>
       <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr"/>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:14:34.870-0500</t>
+        </is>
+      </c>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
@@ -2216,12 +3288,24 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>TPGSOC-1327867</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr"/>
+          <t>TPGSOC-1328093</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:27:32.138-0500</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:12:53.621-0500</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:24:45.273-0500</t>
+        </is>
+      </c>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr"/>
@@ -2230,12 +3314,20 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>TPGSOC-1327810</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr"/>
+          <t>TPGSOC-1328090</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2025-12-30T01:27:25.304-0500</t>
+        </is>
+      </c>
       <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr"/>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2025-12-30T03:08:44.103-0500</t>
+        </is>
+      </c>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr"/>
@@ -2244,11 +3336,19 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>TPGSOC-1327668</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
+          <t>TPGSOC-1327942</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2025-12-29T23:11:29.320-0500</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2025-12-29T23:38:34.632-0500</t>
+        </is>
+      </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
@@ -2258,12 +3358,24 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>TPGSOC-1327174</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr"/>
+          <t>TPGSOC-1327867</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2025-12-29T22:14:42.818-0500</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2025-12-29T23:38:31.337-0500</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2025-12-30T00:02:20.521-0500</t>
+        </is>
+      </c>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
@@ -2272,12 +3384,24 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>TPGSOC-1327100</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr"/>
+          <t>TPGSOC-1327864</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2025-12-29T22:14:22.684-0500</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2025-12-29T23:37:34.834-0500</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2025-12-30T00:01:45.554-0500</t>
+        </is>
+      </c>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
@@ -2286,12 +3410,20 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>TPGSOC-1326106</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr"/>
+          <t>TPGSOC-1327810</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2025-12-29T21:28:47.742-0500</t>
+        </is>
+      </c>
       <c r="C132" t="inlineStr"/>
-      <c r="D132" t="inlineStr"/>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2025-12-29T21:45:42.919-0500</t>
+        </is>
+      </c>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
@@ -2300,11 +3432,19 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>TPGSOC-1324953</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
+          <t>TPGSOC-1327668</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>2025-12-31T04:03:15.646-0500</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2025-12-31T10:37:56.064-0500</t>
+        </is>
+      </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
@@ -2314,11 +3454,19 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>TPGSOC-1324814</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
+          <t>TPGSOC-1327174</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>2025-12-29T11:21:53.651-0500</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2025-12-29T12:12:33.812-0500</t>
+        </is>
+      </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
@@ -2328,11 +3476,19 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>TPGSOC-1324520</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
+          <t>TPGSOC-1327100</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2025-12-29T08:49:51.016-0500</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2025-12-29T09:34:44.539-0500</t>
+        </is>
+      </c>
       <c r="D135" t="inlineStr"/>
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="inlineStr"/>
@@ -2342,7 +3498,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>TPGSOC-1323444</t>
+          <t>TPGSOC-1326106</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -2356,12 +3512,24 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>TPGSOC-1323101</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr"/>
-      <c r="C137" t="inlineStr"/>
-      <c r="D137" t="inlineStr"/>
+          <t>TPGSOC-1324953</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>2025-12-27T07:43:51.377-0500</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2025-12-27T07:53:22.239-0500</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:57:05.462-0500</t>
+        </is>
+      </c>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr"/>
@@ -2370,12 +3538,24 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>TPGSOC-1322647</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" t="inlineStr"/>
-      <c r="D138" t="inlineStr"/>
+          <t>TPGSOC-1324814</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>2025-12-27T06:05:43.775-0500</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2025-12-27T07:36:07.012-0500</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2026-01-07T09:44:10.979-0500</t>
+        </is>
+      </c>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
@@ -2384,12 +3564,24 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>TPGSOC-1322516</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr"/>
+          <t>TPGSOC-1324520</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>2025-12-27T17:14:58.342-0500</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2025-12-27T18:15:59.630-0500</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2025-12-29T22:00:49.669-0500</t>
+        </is>
+      </c>
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
@@ -2398,12 +3590,24 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>TPGSOC-1322095</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr"/>
-      <c r="C140" t="inlineStr"/>
-      <c r="D140" t="inlineStr"/>
+          <t>TPGSOC-1323444</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>2025-12-29T07:07:36.908-0500</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2025-12-29T08:41:38.437-0500</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2025-12-26T19:46:09.269-0500</t>
+        </is>
+      </c>
       <c r="E140" t="inlineStr"/>
       <c r="F140" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
@@ -2412,12 +3616,16 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>TPGSOC-1322058</t>
+          <t>TPGSOC-1323101</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
       <c r="C141" t="inlineStr"/>
-      <c r="D141" t="inlineStr"/>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2025-12-25T05:35:03.573-0500</t>
+        </is>
+      </c>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
       <c r="G141" t="inlineStr"/>
@@ -2426,12 +3634,24 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>TPGSOC-1321940</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr"/>
-      <c r="C142" t="inlineStr"/>
-      <c r="D142" t="inlineStr"/>
+          <t>TPGSOC-1322647</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>2025-12-25T05:10:13.323-0500</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2025-12-25T08:47:40.232-0500</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2026-01-14T22:11:26.800-0500</t>
+        </is>
+      </c>
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
@@ -2440,11 +3660,19 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>TPGSOC-1321279</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr"/>
-      <c r="C143" t="inlineStr"/>
+          <t>TPGSOC-1322516</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>2025-12-24T23:52:34.913-0500</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2025-12-25T08:43:34.656-0500</t>
+        </is>
+      </c>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
       <c r="F143" t="inlineStr"/>
@@ -2454,11 +3682,19 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>TPGSOC-1321120</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr"/>
-      <c r="C144" t="inlineStr"/>
+          <t>TPGSOC-1322095</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>2025-12-24T10:01:55.308-0500</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2025-12-25T16:07:07.303-0500</t>
+        </is>
+      </c>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
@@ -2468,12 +3704,24 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>TPGSOC-1321067</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr"/>
-      <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr"/>
+          <t>TPGSOC-1322058</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>2025-12-24T08:39:45.751-0500</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2025-12-24T12:45:07.416-0500</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2026-01-10T10:26:52.151-0500</t>
+        </is>
+      </c>
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
@@ -2482,12 +3730,24 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>TPGSOC-1320900</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr"/>
-      <c r="C146" t="inlineStr"/>
-      <c r="D146" t="inlineStr"/>
+          <t>TPGSOC-1321940</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>2025-12-24T08:28:48.251-0500</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2025-12-25T14:57:36.937-0500</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:19:57.227-0500</t>
+        </is>
+      </c>
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
@@ -2496,12 +3756,24 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>TPGSOC-1320490</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-      <c r="D147" t="inlineStr"/>
+          <t>TPGSOC-1321279</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>2025-12-24T07:50:56.248-0500</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2025-12-24T13:23:51.657-0500</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:17:10.587-0500</t>
+        </is>
+      </c>
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
@@ -2510,12 +3782,20 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>TPGSOC-1320152</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr"/>
+          <t>TPGSOC-1321120</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>2025-12-23T12:43:13.223-0500</t>
+        </is>
+      </c>
       <c r="C148" t="inlineStr"/>
-      <c r="D148" t="inlineStr"/>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2025-12-24T09:21:28.693-0500</t>
+        </is>
+      </c>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
@@ -2524,12 +3804,24 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>TPGSOC-1320093</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr"/>
-      <c r="C149" t="inlineStr"/>
-      <c r="D149" t="inlineStr"/>
+          <t>TPGSOC-1321067</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>2025-12-23T12:17:12.889-0500</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2025-12-24T09:24:36.498-0500</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2026-01-02T12:13:40.677-0500</t>
+        </is>
+      </c>
       <c r="E149" t="inlineStr"/>
       <c r="F149" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
@@ -2538,11 +3830,19 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>TPGSOC-1320008</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
+          <t>TPGSOC-1320900</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>2025-12-23T10:29:32.200-0500</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2025-12-24T12:02:13.141-0500</t>
+        </is>
+      </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr"/>
@@ -2552,12 +3852,16 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>TPGSOC-1319989</t>
+          <t>TPGSOC-1320490</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
       <c r="C151" t="inlineStr"/>
-      <c r="D151" t="inlineStr"/>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2025-12-23T02:26:01.036-0500</t>
+        </is>
+      </c>
       <c r="E151" t="inlineStr"/>
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
@@ -2566,12 +3870,20 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>TPGSOC-1319903</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr"/>
+          <t>TPGSOC-1320152</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>2025-12-23T04:12:29.538-0500</t>
+        </is>
+      </c>
       <c r="C152" t="inlineStr"/>
-      <c r="D152" t="inlineStr"/>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2025-12-23T08:34:54.659-0500</t>
+        </is>
+      </c>
       <c r="E152" t="inlineStr"/>
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
@@ -2580,12 +3892,24 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>TPGSOC-1319599</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-      <c r="D153" t="inlineStr"/>
+          <t>TPGSOC-1320093</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>2025-12-22T18:10:51.420-0500</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2025-12-22T23:06:53.437-0500</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2026-01-02T00:19:28.602-0500</t>
+        </is>
+      </c>
       <c r="E153" t="inlineStr"/>
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
@@ -2594,12 +3918,16 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>TPGSOC-1319484</t>
+          <t>TPGSOC-1320008</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
       <c r="C154" t="inlineStr"/>
-      <c r="D154" t="inlineStr"/>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2025-12-26T10:19:35.206-0500</t>
+        </is>
+      </c>
       <c r="E154" t="inlineStr"/>
       <c r="F154" t="inlineStr"/>
       <c r="G154" t="inlineStr"/>
@@ -2608,12 +3936,16 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>TPGSOC-1319478</t>
+          <t>TPGSOC-1319989</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
       <c r="C155" t="inlineStr"/>
-      <c r="D155" t="inlineStr"/>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:13:07.366-0500</t>
+        </is>
+      </c>
       <c r="E155" t="inlineStr"/>
       <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
@@ -2622,7 +3954,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>TPGSOC-1319321</t>
+          <t>TPGSOC-1319903</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -2636,12 +3968,24 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>TPGSOC-1319130</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
-      <c r="D157" t="inlineStr"/>
+          <t>TPGSOC-1319599</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>2025-12-22T10:54:34.720-0500</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2025-12-22T23:23:12.284-0500</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2026-01-02T12:12:30.328-0500</t>
+        </is>
+      </c>
       <c r="E157" t="inlineStr"/>
       <c r="F157" t="inlineStr"/>
       <c r="G157" t="inlineStr"/>
@@ -2650,12 +3994,24 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>TPGSOC-1318063</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr"/>
-      <c r="C158" t="inlineStr"/>
-      <c r="D158" t="inlineStr"/>
+          <t>TPGSOC-1319484</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>2025-12-22T11:58:33.770-0500</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2025-12-23T10:33:15.029-0500</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2026-01-02T12:10:39.415-0500</t>
+        </is>
+      </c>
       <c r="E158" t="inlineStr"/>
       <c r="F158" t="inlineStr"/>
       <c r="G158" t="inlineStr"/>
@@ -2664,12 +4020,20 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>TPGSOC-1317999</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr"/>
+          <t>TPGSOC-1319478</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>2025-12-22T09:30:55.248-0500</t>
+        </is>
+      </c>
       <c r="C159" t="inlineStr"/>
-      <c r="D159" t="inlineStr"/>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2025-12-22T15:44:57.849-0500</t>
+        </is>
+      </c>
       <c r="E159" t="inlineStr"/>
       <c r="F159" t="inlineStr"/>
       <c r="G159" t="inlineStr"/>
@@ -2678,12 +4042,24 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>TPGSOC-1317987</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-      <c r="D160" t="inlineStr"/>
+          <t>TPGSOC-1319321</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>2025-12-22T05:18:30.066-0500</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2025-12-22T08:32:03.680-0500</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2025-12-26T08:59:11.854-0500</t>
+        </is>
+      </c>
       <c r="E160" t="inlineStr"/>
       <c r="F160" t="inlineStr"/>
       <c r="G160" t="inlineStr"/>
@@ -2692,12 +4068,24 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>TPGSOC-1317919</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
-      <c r="D161" t="inlineStr"/>
+          <t>TPGSOC-1319130</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>2025-12-22T01:48:23.435-0500</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2025-12-22T08:32:05.848-0500</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2026-01-14T22:08:27.542-0500</t>
+        </is>
+      </c>
       <c r="E161" t="inlineStr"/>
       <c r="F161" t="inlineStr"/>
       <c r="G161" t="inlineStr"/>
@@ -2706,11 +4094,19 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>TPGSOC-1317913</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr"/>
-      <c r="C162" t="inlineStr"/>
+          <t>TPGSOC-1318063</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:26:04.747-0500</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2025-12-21T11:39:45.667-0500</t>
+        </is>
+      </c>
       <c r="D162" t="inlineStr"/>
       <c r="E162" t="inlineStr"/>
       <c r="F162" t="inlineStr"/>
@@ -2720,11 +4116,19 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>TPGSOC-1317770</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr"/>
+          <t>TPGSOC-1317999</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:00:39.821-0500</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:34:12.538-0500</t>
+        </is>
+      </c>
       <c r="D163" t="inlineStr"/>
       <c r="E163" t="inlineStr"/>
       <c r="F163" t="inlineStr"/>
@@ -2734,12 +4138,24 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>TPGSOC-1317453</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr"/>
-      <c r="D164" t="inlineStr"/>
+          <t>TPGSOC-1317987</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>2025-12-21T04:49:04.940-0500</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:42:35.592-0500</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2025-12-26T08:56:21.908-0500</t>
+        </is>
+      </c>
       <c r="E164" t="inlineStr"/>
       <c r="F164" t="inlineStr"/>
       <c r="G164" t="inlineStr"/>
@@ -2748,11 +4164,19 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>TPGSOC-1317447</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr"/>
-      <c r="C165" t="inlineStr"/>
+          <t>TPGSOC-1317919</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>2025-12-21T06:45:35.174-0500</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:34:16.347-0500</t>
+        </is>
+      </c>
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr"/>
       <c r="F165" t="inlineStr"/>
@@ -2762,12 +4186,24 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>TPGSOC-1317377</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-      <c r="D166" t="inlineStr"/>
+          <t>TPGSOC-1317913</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>2025-12-21T06:30:24.072-0500</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2025-12-21T08:34:19.324-0500</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2025-12-26T08:55:02.541-0500</t>
+        </is>
+      </c>
       <c r="E166" t="inlineStr"/>
       <c r="F166" t="inlineStr"/>
       <c r="G166" t="inlineStr"/>
@@ -2776,11 +4212,19 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>TPGSOC-1317376</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr"/>
-      <c r="C167" t="inlineStr"/>
+          <t>TPGSOC-1317770</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>2025-12-20T09:18:01.789-0500</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2025-12-20T12:30:49.461-0500</t>
+        </is>
+      </c>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="inlineStr"/>
       <c r="F167" t="inlineStr"/>
@@ -2790,11 +4234,19 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>TPGSOC-1317172</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
+          <t>TPGSOC-1317453</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>2025-12-21T12:55:14.039-0500</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2025-12-21T22:47:01.070-0500</t>
+        </is>
+      </c>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr"/>
       <c r="F168" t="inlineStr"/>
@@ -2804,12 +4256,20 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>TPGSOC-1316870</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr"/>
+          <t>TPGSOC-1317447</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>2025-12-20T09:52:57.140-0500</t>
+        </is>
+      </c>
       <c r="C169" t="inlineStr"/>
-      <c r="D169" t="inlineStr"/>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2025-12-21T22:50:55.287-0500</t>
+        </is>
+      </c>
       <c r="E169" t="inlineStr"/>
       <c r="F169" t="inlineStr"/>
       <c r="G169" t="inlineStr"/>
@@ -2818,12 +4278,24 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>TPGSOC-1316855</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-      <c r="D170" t="inlineStr"/>
+          <t>TPGSOC-1317377</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>2025-12-20T09:51:49.576-0500</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2025-12-20T12:17:36.617-0500</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2026-01-14T10:09:57.013-0500</t>
+        </is>
+      </c>
       <c r="E170" t="inlineStr"/>
       <c r="F170" t="inlineStr"/>
       <c r="G170" t="inlineStr"/>
@@ -2832,12 +4304,20 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>TPGSOC-1316100</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr"/>
+          <t>TPGSOC-1317376</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>2025-12-20T09:50:47.171-0500</t>
+        </is>
+      </c>
       <c r="C171" t="inlineStr"/>
-      <c r="D171" t="inlineStr"/>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2025-12-20T10:57:05.047-0500</t>
+        </is>
+      </c>
       <c r="E171" t="inlineStr"/>
       <c r="F171" t="inlineStr"/>
       <c r="G171" t="inlineStr"/>
@@ -2846,12 +4326,24 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>TPGSOC-1315860</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr"/>
-      <c r="C172" t="inlineStr"/>
-      <c r="D172" t="inlineStr"/>
+          <t>TPGSOC-1317172</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>2025-12-20T04:10:30.487-0500</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2025-12-20T06:23:05.021-0500</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2025-12-26T08:53:50.721-0500</t>
+        </is>
+      </c>
       <c r="E172" t="inlineStr"/>
       <c r="F172" t="inlineStr"/>
       <c r="G172" t="inlineStr"/>
@@ -2860,12 +4352,24 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>TPGSOC-1315805</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr"/>
-      <c r="C173" t="inlineStr"/>
-      <c r="D173" t="inlineStr"/>
+          <t>TPGSOC-1316870</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>2025-12-19T07:41:04.593-0500</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2025-12-19T07:48:39.275-0500</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2026-01-14T08:58:13.818-0500</t>
+        </is>
+      </c>
       <c r="E173" t="inlineStr"/>
       <c r="F173" t="inlineStr"/>
       <c r="G173" t="inlineStr"/>
@@ -2874,12 +4378,24 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>TPGSOC-1315793</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr"/>
-      <c r="D174" t="inlineStr"/>
+          <t>TPGSOC-1316855</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>2025-12-19T08:18:29.216-0500</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2025-12-19T10:58:54.977-0500</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2025-12-26T10:14:07.881-0500</t>
+        </is>
+      </c>
       <c r="E174" t="inlineStr"/>
       <c r="F174" t="inlineStr"/>
       <c r="G174" t="inlineStr"/>
@@ -2888,11 +4404,19 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>TPGSOC-1315587</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
+          <t>TPGSOC-1316100</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>2025-12-20T02:43:04.040-0500</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2025-12-20T06:23:07.935-0500</t>
+        </is>
+      </c>
       <c r="D175" t="inlineStr"/>
       <c r="E175" t="inlineStr"/>
       <c r="F175" t="inlineStr"/>
@@ -2902,12 +4426,20 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>TPGSOC-1315571</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr"/>
+          <t>TPGSOC-1315860</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>2025-12-18T10:15:16.463-0500</t>
+        </is>
+      </c>
       <c r="C176" t="inlineStr"/>
-      <c r="D176" t="inlineStr"/>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2025-12-20T12:06:50.659-0500</t>
+        </is>
+      </c>
       <c r="E176" t="inlineStr"/>
       <c r="F176" t="inlineStr"/>
       <c r="G176" t="inlineStr"/>
@@ -2916,12 +4448,20 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>TPGSOC-1315346</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr"/>
+          <t>TPGSOC-1315805</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>2025-12-18T05:54:06.280-0500</t>
+        </is>
+      </c>
       <c r="C177" t="inlineStr"/>
-      <c r="D177" t="inlineStr"/>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2025-12-18T06:23:20.332-0500</t>
+        </is>
+      </c>
       <c r="E177" t="inlineStr"/>
       <c r="F177" t="inlineStr"/>
       <c r="G177" t="inlineStr"/>
@@ -2930,17 +4470,121 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>TPGSOC-1314937</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr"/>
-      <c r="C178" t="inlineStr"/>
-      <c r="D178" t="inlineStr"/>
+          <t>TPGSOC-1315793</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2025-12-18T07:26:46.186-0500</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>2025-12-18T09:07:08.385-0500</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2025-12-26T10:11:12.346-0500</t>
+        </is>
+      </c>
       <c r="E178" t="inlineStr"/>
       <c r="F178" t="inlineStr"/>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="inlineStr"/>
     </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>TPGSOC-1315587</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2025-12-18T10:19:12.230-0500</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>2025-12-18T11:03:59.252-0500</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2026-01-07T09:46:27.873-0500</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="inlineStr"/>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>TPGSOC-1315571</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2025-12-18T02:29:00.426-0500</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>2025-12-18T09:01:37.601-0500</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr"/>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>TPGSOC-1315346</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>2025-12-18T05:24:28.631-0500</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2025-12-19T09:37:07.402-0500</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>TPGSOC-1314937</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2025-12-17T12:42:01.411-0500</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2025-12-17T15:26:19.314-0500</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr"/>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="inlineStr"/>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>